<commit_message>
Revised L1 for possible 2A output, cleaner fill zones, fabrication outputs
</commit_message>
<xml_diff>
--- a/Hardware/Arch_Bridge/Current Limit calculator.xlsx
+++ b/Hardware/Arch_Bridge/Current Limit calculator.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t xml:space="preserve">A</t>
   </si>
@@ -49,6 +49,9 @@
     <t xml:space="preserve">Trip</t>
   </si>
   <si>
+    <t xml:space="preserve">Trip_Tick</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vmax</t>
   </si>
   <si>
@@ -56,6 +59,9 @@
   </si>
   <si>
     <t xml:space="preserve">Div/V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Div/A</t>
   </si>
   <si>
     <t xml:space="preserve">Count</t>
@@ -167,13 +173,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J23" activeCellId="0" sqref="J23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L30" activeCellId="0" sqref="L30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -238,7 +244,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="n">
@@ -248,7 +254,7 @@
         <f aca="false">B3</f>
         <v>0.001</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="2" t="n">
@@ -448,211 +454,295 @@
         <f aca="false">H8/H2</f>
         <v>2.41516725033209</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="J9" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B10" s="0" t="n">
+        <f aca="false">B9*B14</f>
+        <v>319.674513222899</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <f aca="false">C9*C14</f>
+        <v>319.354838709677</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <f aca="false">D9*D14</f>
+        <v>319.03580290677</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <f aca="false">F9*F14</f>
+        <v>3196.74513222899</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <f aca="false">G9*G14</f>
+        <v>3193.54838709677</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <f aca="false">H9*H14</f>
+        <v>3190.3580290677</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="n">
         <v>3.1</v>
       </c>
-      <c r="C11" s="0" t="n">
-        <f aca="false">B11</f>
+      <c r="C12" s="1" t="n">
+        <f aca="false">B12</f>
         <v>3.1</v>
       </c>
-      <c r="D11" s="0" t="n">
-        <f aca="false">C11</f>
+      <c r="D12" s="1" t="n">
+        <f aca="false">C12</f>
         <v>3.1</v>
       </c>
-      <c r="E11" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <f aca="false">D11</f>
+      <c r="E12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <f aca="false">D12</f>
         <v>3.1</v>
       </c>
-      <c r="G11" s="0" t="n">
-        <f aca="false">F11</f>
+      <c r="G12" s="1" t="n">
+        <f aca="false">F12</f>
         <v>3.1</v>
       </c>
-      <c r="H11" s="0" t="n">
-        <f aca="false">G11</f>
+      <c r="H12" s="1" t="n">
+        <f aca="false">G12</f>
         <v>3.1</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="0" t="n">
+      <c r="J12" s="0" t="n">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="n">
         <v>4095</v>
       </c>
-      <c r="C12" s="0" t="n">
-        <f aca="false">B12</f>
+      <c r="C13" s="1" t="n">
+        <f aca="false">B13</f>
         <v>4095</v>
       </c>
-      <c r="D12" s="0" t="n">
-        <f aca="false">C12</f>
+      <c r="D13" s="1" t="n">
+        <f aca="false">C13</f>
         <v>4095</v>
       </c>
-      <c r="E12" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <f aca="false">D12</f>
+      <c r="E13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <f aca="false">D13</f>
         <v>4095</v>
       </c>
-      <c r="G12" s="0" t="n">
-        <f aca="false">F12</f>
+      <c r="G13" s="1" t="n">
+        <f aca="false">F13</f>
         <v>4095</v>
       </c>
-      <c r="H12" s="0" t="n">
-        <f aca="false">G12</f>
+      <c r="H13" s="1" t="n">
+        <f aca="false">G13</f>
         <v>4095</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <f aca="false">B12/B11</f>
+      <c r="J13" s="0" t="n">
+        <v>4095</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <f aca="false">B13/B12</f>
         <v>1320.96774193548</v>
       </c>
-      <c r="C13" s="0" t="n">
-        <f aca="false">C12/C11</f>
+      <c r="C14" s="1" t="n">
+        <f aca="false">C13/C12</f>
         <v>1320.96774193548</v>
       </c>
-      <c r="D13" s="0" t="n">
-        <f aca="false">D12/D11</f>
+      <c r="D14" s="1" t="n">
+        <f aca="false">D13/D12</f>
         <v>1320.96774193548</v>
       </c>
-      <c r="E13" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <f aca="false">F12/F11</f>
+      <c r="E14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <f aca="false">F13/F12</f>
         <v>1320.96774193548</v>
       </c>
-      <c r="G13" s="0" t="n">
-        <f aca="false">G12/G11</f>
+      <c r="G14" s="1" t="n">
+        <f aca="false">G13/G12</f>
         <v>1320.96774193548</v>
       </c>
-      <c r="H13" s="0" t="n">
-        <f aca="false">H12/H11</f>
+      <c r="H14" s="1" t="n">
+        <f aca="false">H13/H12</f>
         <v>1320.96774193548</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <f aca="false">ROUND(B12/B11*B6,0)</f>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1" t="n">
+        <f aca="false">J13/J12</f>
+        <v>1320.96774193548</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <f aca="false">B13/B9</f>
+        <v>16921.4706818182</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <f aca="false">C13/C9</f>
+        <v>16938.4090909091</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <f aca="false">D13/D9</f>
+        <v>16955.3475</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <f aca="false">F13/F9</f>
+        <v>1692.14706818182</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <f aca="false">G13/G9</f>
+        <v>1693.84090909091</v>
+      </c>
+      <c r="H15" s="1" t="n">
+        <f aca="false">H13/H9</f>
+        <v>1695.53475</v>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1" t="n">
+        <f aca="false">J13/J9</f>
+        <v>819</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <f aca="false">ROUND(B13/B12*B6,0)</f>
         <v>3603</v>
       </c>
-      <c r="C14" s="0" t="n">
-        <f aca="false">ROUND(C12/C11*C6,0)</f>
+      <c r="C16" s="1" t="n">
+        <f aca="false">ROUND(C13/C12*C6,0)</f>
         <v>3606</v>
       </c>
-      <c r="D14" s="0" t="n">
-        <f aca="false">ROUND(D12/D11*D6,0)</f>
+      <c r="D16" s="1" t="n">
+        <f aca="false">ROUND(D13/D12*D6,0)</f>
         <v>3610</v>
       </c>
-      <c r="E14" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <f aca="false">ROUND(F12/F11*F6,0)</f>
+      <c r="E16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <f aca="false">ROUND(F13/F12*F6,0)</f>
         <v>3603</v>
       </c>
-      <c r="G14" s="0" t="n">
-        <f aca="false">ROUND(G12/G11*G6,0)</f>
+      <c r="G16" s="1" t="n">
+        <f aca="false">ROUND(G13/G12*G6,0)</f>
         <v>3606</v>
       </c>
-      <c r="H14" s="0" t="n">
-        <f aca="false">ROUND(H12/H11*H6,0)</f>
+      <c r="H16" s="1" t="n">
+        <f aca="false">ROUND(H13/H12*H6,0)</f>
         <v>3610</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B20" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="C20" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="D20" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="E20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="H20" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="I20" s="0" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
-        <v>3300</v>
-      </c>
-      <c r="B21" s="1" t="n">
-        <v>3300</v>
-      </c>
-      <c r="C21" s="1" t="n">
-        <v>3300</v>
-      </c>
-      <c r="D21" s="1" t="n">
-        <v>3300</v>
-      </c>
-      <c r="E21" s="1" t="n">
-        <v>3300</v>
-      </c>
-      <c r="H21" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="I21" s="0" t="n">
-        <f aca="false">H21</f>
-        <v>16</v>
+      <c r="L16" s="0" t="n">
+        <f aca="false">38*8</f>
+        <v>304</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
-        <f aca="false">A20/A21</f>
+        <v>5</v>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="H22" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="I22" s="1" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="n">
+        <v>3300</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>3300</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>3300</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>3300</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <v>3300</v>
+      </c>
+      <c r="H23" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="I23" s="1" t="n">
+        <f aca="false">H23</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="n">
+        <f aca="false">A22/A23</f>
         <v>0.00151515151515152</v>
       </c>
-      <c r="B22" s="1" t="n">
-        <f aca="false">B20/B21</f>
+      <c r="B24" s="1" t="n">
+        <f aca="false">B22/B23</f>
         <v>0.00212121212121212</v>
       </c>
-      <c r="C22" s="1" t="n">
-        <f aca="false">C20/C21</f>
+      <c r="C24" s="1" t="n">
+        <f aca="false">C22/C23</f>
         <v>0.00363636363636364</v>
       </c>
-      <c r="D22" s="1" t="n">
-        <f aca="false">D20/D21</f>
+      <c r="D24" s="1" t="n">
+        <f aca="false">D22/D23</f>
         <v>0.00454545454545455</v>
       </c>
-      <c r="E22" s="1" t="n">
-        <f aca="false">E20/E21</f>
+      <c r="E24" s="1" t="n">
+        <f aca="false">E22/E23</f>
         <v>0.00545454545454546</v>
       </c>
-      <c r="H22" s="0" t="n">
-        <f aca="false">H20/H21</f>
+      <c r="H24" s="1" t="n">
+        <f aca="false">H22/H23</f>
         <v>0.75</v>
       </c>
-      <c r="I22" s="0" t="n">
-        <f aca="false">I20/I21</f>
+      <c r="I24" s="1" t="n">
+        <f aca="false">I22/I23</f>
         <v>0.9375</v>
       </c>
-      <c r="J22" s="0" t="s">
-        <v>13</v>
+      <c r="J24" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Power modes partially implemented. Railsync output H bridge handled a test waveform correctly.
</commit_message>
<xml_diff>
--- a/Hardware/Arch_Bridge/Current Limit calculator.xlsx
+++ b/Hardware/Arch_Bridge/Current Limit calculator.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
   <si>
     <t xml:space="preserve">A</t>
   </si>
@@ -67,7 +67,13 @@
     <t xml:space="preserve">Count</t>
   </si>
   <si>
-    <t xml:space="preserve">amps</t>
+    <t xml:space="preserve">Div/(A*100)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count * 100000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mA</t>
   </si>
 </sst>
 </file>
@@ -173,13 +179,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L30" activeCellId="0" sqref="L30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -454,9 +460,6 @@
         <f aca="false">H8/H2</f>
         <v>2.41516725033209</v>
       </c>
-      <c r="J9" s="0" t="n">
-        <v>5</v>
-      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
@@ -517,9 +520,6 @@
         <f aca="false">G12</f>
         <v>3.1</v>
       </c>
-      <c r="J12" s="0" t="n">
-        <v>3.1</v>
-      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
@@ -551,9 +551,6 @@
         <f aca="false">G13</f>
         <v>4095</v>
       </c>
-      <c r="J13" s="0" t="n">
-        <v>4095</v>
-      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
@@ -587,10 +584,7 @@
         <v>1320.96774193548</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="1" t="n">
-        <f aca="false">J13/J12</f>
-        <v>1320.96774193548</v>
-      </c>
+      <c r="J14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
@@ -624,10 +618,7 @@
         <v>1695.53475</v>
       </c>
       <c r="I15" s="1"/>
-      <c r="J15" s="1" t="n">
-        <f aca="false">J13/J9</f>
-        <v>819</v>
-      </c>
+      <c r="J15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
@@ -660,90 +651,105 @@
         <f aca="false">ROUND(H13/H12*H6,0)</f>
         <v>3610</v>
       </c>
-      <c r="L16" s="0" t="n">
-        <f aca="false">38*8</f>
-        <v>304</v>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <f aca="false">B15*100</f>
+        <v>1692147.06818182</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <f aca="false">C15*100</f>
+        <v>1693840.90909091</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <f aca="false">D15*100</f>
+        <v>1695534.75</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <f aca="false">F15*100</f>
+        <v>169214.706818182</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <f aca="false">G15*100</f>
+        <v>169384.090909091</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <f aca="false">H15*100</f>
+        <v>169553.475</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <f aca="false">B20*100000</f>
+        <v>6000000</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <f aca="false">C20*100000</f>
+        <v>12000000</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <f aca="false">D20*100000</f>
+        <v>20000000</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
-        <v>5</v>
+      <c r="A22" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B22" s="1" t="n">
-        <v>7</v>
+        <f aca="false">B21/B19</f>
+        <v>3.54579109157863</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>12</v>
+        <f aca="false">C21/C19</f>
+        <v>7.08449060097411</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="E22" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="H22" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="I22" s="1" t="n">
-        <v>15</v>
-      </c>
+        <f aca="false">D21/D19</f>
+        <v>11.7956886463106</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
-        <v>3300</v>
-      </c>
-      <c r="B23" s="1" t="n">
-        <v>3300</v>
-      </c>
-      <c r="C23" s="1" t="n">
-        <v>3300</v>
-      </c>
-      <c r="D23" s="1" t="n">
-        <v>3300</v>
-      </c>
-      <c r="E23" s="1" t="n">
-        <v>3300</v>
-      </c>
-      <c r="H23" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="I23" s="1" t="n">
-        <f aca="false">H23</f>
-        <v>16</v>
-      </c>
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
-        <f aca="false">A22/A23</f>
-        <v>0.00151515151515152</v>
-      </c>
-      <c r="B24" s="1" t="n">
-        <f aca="false">B22/B23</f>
-        <v>0.00212121212121212</v>
-      </c>
-      <c r="C24" s="1" t="n">
-        <f aca="false">C22/C23</f>
-        <v>0.00363636363636364</v>
-      </c>
-      <c r="D24" s="1" t="n">
-        <f aca="false">D22/D23</f>
-        <v>0.00454545454545455</v>
-      </c>
-      <c r="E24" s="1" t="n">
-        <f aca="false">E22/E23</f>
-        <v>0.00545454545454546</v>
-      </c>
-      <c r="H24" s="1" t="n">
-        <f aca="false">H22/H23</f>
-        <v>0.75</v>
-      </c>
-      <c r="I24" s="1" t="n">
-        <f aca="false">I22/I23</f>
-        <v>0.9375</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Adjusted R15 value and ADC code to make railsync current source work correctly. 0-208mA availabe.
</commit_message>
<xml_diff>
--- a/Hardware/Arch_Bridge/Current Limit calculator.xlsx
+++ b/Hardware/Arch_Bridge/Current Limit calculator.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t xml:space="preserve">A</t>
   </si>
@@ -67,10 +67,13 @@
     <t xml:space="preserve">Count</t>
   </si>
   <si>
-    <t xml:space="preserve">Div/(A*100)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Count * 100000</t>
+    <t xml:space="preserve">Div/(A*1000)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count * 1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count * 1000000</t>
   </si>
   <si>
     <t xml:space="preserve">mA</t>
@@ -179,13 +182,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29:B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -327,7 +330,6 @@
         <v>909.09</v>
       </c>
       <c r="G5" s="1" t="n">
-        <f aca="false">C5/10</f>
         <v>910</v>
       </c>
       <c r="H5" s="1" t="n">
@@ -462,30 +464,30 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <f aca="false">B9*B14</f>
         <v>319.674513222899</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <f aca="false">C9*C14</f>
-        <v>319.354838709677</v>
-      </c>
-      <c r="D10" s="0" t="n">
+        <v>319.354838709676</v>
+      </c>
+      <c r="D10" s="1" t="n">
         <f aca="false">D9*D14</f>
         <v>319.03580290677</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="1" t="n">
         <f aca="false">F9*F14</f>
         <v>3196.74513222899</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <f aca="false">G9*G14</f>
-        <v>3193.54838709677</v>
-      </c>
-      <c r="H10" s="0" t="n">
+        <v>3193.54838709676</v>
+      </c>
+      <c r="H10" s="1" t="n">
         <f aca="false">H9*H14</f>
         <v>3190.3580290677</v>
       </c>
@@ -653,63 +655,73 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="0" t="n">
-        <f aca="false">B15*100</f>
-        <v>1692147.06818182</v>
-      </c>
-      <c r="C19" s="0" t="n">
-        <f aca="false">C15*100</f>
-        <v>1693840.90909091</v>
-      </c>
-      <c r="D19" s="0" t="n">
-        <f aca="false">D15*100</f>
-        <v>1695534.75</v>
-      </c>
-      <c r="F19" s="0" t="n">
-        <f aca="false">F15*100</f>
-        <v>169214.706818182</v>
-      </c>
-      <c r="G19" s="0" t="n">
-        <f aca="false">G15*100</f>
-        <v>169384.090909091</v>
-      </c>
-      <c r="H19" s="0" t="n">
-        <f aca="false">H15*100</f>
-        <v>169553.475</v>
+      <c r="B19" s="1" t="n">
+        <f aca="false">ROUND(B15*1000,0)</f>
+        <v>16921471</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <f aca="false">ROUND(C15*1000,0)</f>
+        <v>16938409</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <f aca="false">ROUND(D15*1000,0)</f>
+        <v>16955348</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1" t="n">
+        <f aca="false">ROUND(F15*1000,0)</f>
+        <v>1692147</v>
+      </c>
+      <c r="G19" s="1" t="n">
+        <f aca="false">ROUND(G15*1000,0)</f>
+        <v>1693841</v>
+      </c>
+      <c r="H19" s="1" t="n">
+        <f aca="false">ROUND(H15*1000,0)</f>
+        <v>1695535</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="C20" s="0" t="n">
-        <v>120</v>
-      </c>
-      <c r="D20" s="0" t="n">
+      <c r="C20" s="1" t="n">
+        <v>3541</v>
+      </c>
+      <c r="D20" s="1" t="n">
         <v>200</v>
       </c>
+      <c r="F20" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>3388</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>240</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="0" t="n">
-        <f aca="false">B20*100000</f>
-        <v>6000000</v>
-      </c>
-      <c r="C21" s="0" t="n">
-        <f aca="false">C20*100000</f>
-        <v>12000000</v>
-      </c>
-      <c r="D21" s="0" t="n">
-        <f aca="false">D20*100000</f>
-        <v>20000000</v>
+      <c r="B21" s="1" t="n">
+        <f aca="false">B20*1000</f>
+        <v>60000</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <f aca="false">C20*1000</f>
+        <v>3541000</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <f aca="false">D20*1000</f>
+        <v>200000</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -717,28 +729,60 @@
         <v>17</v>
       </c>
       <c r="B22" s="1" t="n">
-        <f aca="false">B21/B19</f>
-        <v>3.54579109157863</v>
+        <f aca="false">B20*1000000</f>
+        <v>60000000</v>
       </c>
       <c r="C22" s="1" t="n">
-        <f aca="false">C21/C19</f>
-        <v>7.08449060097411</v>
+        <f aca="false">C20*1000000</f>
+        <v>3541000000</v>
       </c>
       <c r="D22" s="1" t="n">
-        <f aca="false">D21/D19</f>
-        <v>11.7956886463106</v>
+        <f aca="false">D20*1000000</f>
+        <v>200000000</v>
       </c>
       <c r="E22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
+      <c r="F22" s="1" t="n">
+        <f aca="false">F20*1000000</f>
+        <v>60000000</v>
+      </c>
+      <c r="G22" s="1" t="n">
+        <f aca="false">G20*1000000</f>
+        <v>3388000000</v>
+      </c>
+      <c r="H22" s="1" t="n">
+        <f aca="false">H20*1000000</f>
+        <v>240000000</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
+      <c r="A23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <f aca="false">B22/B19</f>
+        <v>3.54579102490558</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <f aca="false">C22/C19</f>
+        <v>209.051511272399</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <f aca="false">D22/D19</f>
+        <v>11.7956882984649</v>
+      </c>
       <c r="E23" s="1"/>
-      <c r="H23" s="1"/>
+      <c r="F23" s="1" t="n">
+        <f aca="false">F22/F19</f>
+        <v>35.4579123444949</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <f aca="false">G22/G19</f>
+        <v>2000.18773899085</v>
+      </c>
+      <c r="H23" s="1" t="n">
+        <f aca="false">H22/H19</f>
+        <v>141.548242884989</v>
+      </c>
       <c r="I23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -749,7 +793,16 @@
       <c r="E24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Changed ADC calculations to be x1000 instead of x1000000 so the values fit int32_t instead of int64_t.
</commit_message>
<xml_diff>
--- a/Hardware/Arch_Bridge/Current Limit calculator.xlsx
+++ b/Hardware/Arch_Bridge/Current Limit calculator.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t xml:space="preserve">A</t>
   </si>
@@ -64,6 +64,12 @@
     <t xml:space="preserve">Div/A</t>
   </si>
   <si>
+    <t xml:space="preserve">div/mA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Div/mA</t>
+  </si>
+  <si>
     <t xml:space="preserve">Count</t>
   </si>
   <si>
@@ -77,6 +83,15 @@
   </si>
   <si>
     <t xml:space="preserve">mA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int16_t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int32_t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int64_t</t>
   </si>
 </sst>
 </file>
@@ -182,13 +197,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29:B32"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.88"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -627,84 +645,95 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="n">
+        <f aca="false">B15/1000</f>
+        <v>16.9214706818182</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <f aca="false">C15/1000</f>
+        <v>16.9384090909091</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <f aca="false">D15/1000</f>
+        <v>16.9553475</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <f aca="false">F15/1000</f>
+        <v>1.69214706818182</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <f aca="false">G15/1000</f>
+        <v>1.69384090909091</v>
+      </c>
+      <c r="H16" s="1" t="n">
+        <f aca="false">H15/1000</f>
+        <v>1.69553475</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="n">
         <f aca="false">ROUND(B13/B12*B6,0)</f>
         <v>3603</v>
       </c>
-      <c r="C16" s="1" t="n">
+      <c r="C17" s="1" t="n">
         <f aca="false">ROUND(C13/C12*C6,0)</f>
         <v>3606</v>
       </c>
-      <c r="D16" s="1" t="n">
+      <c r="D17" s="1" t="n">
         <f aca="false">ROUND(D13/D12*D6,0)</f>
         <v>3610</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="1" t="n">
+      <c r="E17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="1" t="n">
         <f aca="false">ROUND(F13/F12*F6,0)</f>
         <v>3603</v>
       </c>
-      <c r="G16" s="1" t="n">
+      <c r="G17" s="1" t="n">
         <f aca="false">ROUND(G13/G12*G6,0)</f>
         <v>3606</v>
       </c>
-      <c r="H16" s="1" t="n">
+      <c r="H17" s="1" t="n">
         <f aca="false">ROUND(H13/H12*H6,0)</f>
         <v>3610</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="1" t="n">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="1" t="n">
         <f aca="false">ROUND(B15*1000,0)</f>
         <v>16921471</v>
       </c>
-      <c r="C19" s="1" t="n">
+      <c r="C20" s="1" t="n">
         <f aca="false">ROUND(C15*1000,0)</f>
         <v>16938409</v>
       </c>
-      <c r="D19" s="1" t="n">
+      <c r="D20" s="1" t="n">
         <f aca="false">ROUND(D15*1000,0)</f>
         <v>16955348</v>
       </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1" t="n">
+      <c r="E20" s="1"/>
+      <c r="F20" s="1" t="n">
         <f aca="false">ROUND(F15*1000,0)</f>
         <v>1692147</v>
       </c>
-      <c r="G19" s="1" t="n">
+      <c r="G20" s="1" t="n">
         <f aca="false">ROUND(G15*1000,0)</f>
         <v>1693841</v>
       </c>
-      <c r="H19" s="1" t="n">
+      <c r="H20" s="1" t="n">
         <f aca="false">ROUND(H15*1000,0)</f>
         <v>1695535</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="C20" s="1" t="n">
-        <v>3541</v>
-      </c>
-      <c r="D20" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="F20" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="G20" s="0" t="n">
-        <v>3388</v>
-      </c>
-      <c r="H20" s="0" t="n">
-        <v>240</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -712,86 +741,112 @@
         <v>16</v>
       </c>
       <c r="B21" s="1" t="n">
-        <f aca="false">B20*1000</f>
-        <v>60000</v>
+        <v>60</v>
       </c>
       <c r="C21" s="1" t="n">
-        <f aca="false">C20*1000</f>
-        <v>3541000</v>
+        <v>3650</v>
       </c>
       <c r="D21" s="1" t="n">
-        <f aca="false">D20*1000</f>
-        <v>200000</v>
+        <v>4095</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>3388</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>4095</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B22" s="1" t="n">
-        <f aca="false">B20*1000000</f>
-        <v>60000000</v>
+        <f aca="false">B21*1000</f>
+        <v>60000</v>
       </c>
       <c r="C22" s="1" t="n">
-        <f aca="false">C20*1000000</f>
-        <v>3541000000</v>
+        <f aca="false">C21*1000</f>
+        <v>3650000</v>
       </c>
       <c r="D22" s="1" t="n">
-        <f aca="false">D20*1000000</f>
-        <v>200000000</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1" t="n">
-        <f aca="false">F20*1000000</f>
-        <v>60000000</v>
-      </c>
-      <c r="G22" s="1" t="n">
-        <f aca="false">G20*1000000</f>
-        <v>3388000000</v>
-      </c>
-      <c r="H22" s="1" t="n">
-        <f aca="false">H20*1000000</f>
-        <v>240000000</v>
+        <f aca="false">D21*1000</f>
+        <v>4095000</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <f aca="false">F21*1000</f>
+        <v>60000</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <f aca="false">G21*1000</f>
+        <v>3388000</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <f aca="false">H21*1000</f>
+        <v>4095000</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B23" s="1" t="n">
-        <f aca="false">B22/B19</f>
-        <v>3.54579102490558</v>
+        <f aca="false">B21*1000000</f>
+        <v>60000000</v>
       </c>
       <c r="C23" s="1" t="n">
-        <f aca="false">C22/C19</f>
-        <v>209.051511272399</v>
+        <f aca="false">C21*1000000</f>
+        <v>3650000000</v>
       </c>
       <c r="D23" s="1" t="n">
-        <f aca="false">D22/D19</f>
-        <v>11.7956882984649</v>
+        <f aca="false">D21*1000000</f>
+        <v>4095000000</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="n">
-        <f aca="false">F22/F19</f>
+        <f aca="false">F21*1000000</f>
+        <v>60000000</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <f aca="false">G21*1000000</f>
+        <v>3388000000</v>
+      </c>
+      <c r="H23" s="1" t="n">
+        <f aca="false">H21*1000000</f>
+        <v>4095000000</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="1" t="n">
+        <f aca="false">B23/B20</f>
+        <v>3.54579102490558</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <f aca="false">C23/C20</f>
+        <v>215.486590269488</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <f aca="false">D23/D20</f>
+        <v>241.516717911069</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1" t="n">
+        <f aca="false">F23/F20</f>
         <v>35.4579123444949</v>
       </c>
-      <c r="G23" s="1" t="n">
-        <f aca="false">G22/G19</f>
+      <c r="G24" s="1" t="n">
+        <f aca="false">G23/G20</f>
         <v>2000.18773899085</v>
       </c>
-      <c r="H23" s="1" t="n">
-        <f aca="false">H22/H19</f>
-        <v>141.548242884989</v>
-      </c>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="H24" s="1"/>
+      <c r="H24" s="1" t="n">
+        <f aca="false">H23/H20</f>
+        <v>2415.16689422513</v>
+      </c>
       <c r="I24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -802,7 +857,134 @@
       <c r="E25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="1" t="n">
+        <f aca="false">B22</f>
+        <v>60000</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <f aca="false">C22</f>
+        <v>3650000</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <f aca="false">D22</f>
+        <v>4095000</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1" t="n">
+        <f aca="false">F22</f>
+        <v>60000</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <f aca="false">G22</f>
+        <v>3388000</v>
+      </c>
+      <c r="H26" s="1" t="n">
+        <f aca="false">H22</f>
+        <v>4095000</v>
+      </c>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="0" t="str">
+        <f aca="false">IF(B26&gt;(2^15),"OVF","OK")</f>
+        <v>OVF</v>
+      </c>
+      <c r="C27" s="0" t="str">
+        <f aca="false">IF(C26&gt;(2^15),"OVF","OK")</f>
+        <v>OVF</v>
+      </c>
+      <c r="D27" s="0" t="str">
+        <f aca="false">IF(D26&gt;(2^15),"OVF","OK")</f>
+        <v>OVF</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <f aca="false">2^15</f>
+        <v>32768</v>
+      </c>
+      <c r="F27" s="0" t="str">
+        <f aca="false">IF(F26&gt;(2^15),"OVF","OK")</f>
+        <v>OVF</v>
+      </c>
+      <c r="G27" s="0" t="str">
+        <f aca="false">IF(G26&gt;(2^15),"OVF","OK")</f>
+        <v>OVF</v>
+      </c>
+      <c r="H27" s="0" t="str">
+        <f aca="false">IF(H26&gt;(2^15),"OVF","OK")</f>
+        <v>OVF</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="0" t="str">
+        <f aca="false">IF(B26&gt;(2^31),"OVF","OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="C28" s="0" t="str">
+        <f aca="false">IF(C26&gt;(2^31),"OVF","OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="D28" s="0" t="str">
+        <f aca="false">IF(D26&gt;(2^31),"OVF","OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <f aca="false">2^31</f>
+        <v>2147483648</v>
+      </c>
+      <c r="F28" s="0" t="str">
+        <f aca="false">IF(F26&gt;(2^31),"OVF","OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="G28" s="0" t="str">
+        <f aca="false">IF(G26&gt;(2^31),"OVF","OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="H28" s="0" t="str">
+        <f aca="false">IF(H26&gt;(2^31),"OVF","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="0" t="str">
+        <f aca="false">IF(B26&gt;(2^63),"OVF","OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="C29" s="0" t="str">
+        <f aca="false">IF(C26&gt;(2^63),"OVF","OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="D29" s="0" t="str">
+        <f aca="false">IF(D26&gt;(2^63),"OVF","OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <f aca="false">2^63</f>
+        <v>9.22337203685478E+018</v>
+      </c>
+      <c r="F29" s="0" t="str">
+        <f aca="false">IF(F26&gt;(2^63),"OVF","OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="G29" s="0" t="str">
+        <f aca="false">IF(G26&gt;(2^63),"OVF","OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="H29" s="0" t="str">
+        <f aca="false">IF(H26&gt;(2^63),"OVF","OK")</f>
+        <v>OK</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Added Railsync voltage monitoring circuit, stabilizer cap. Updated BOM with new parts.
</commit_message>
<xml_diff>
--- a/Hardware/Arch_Bridge/Current Limit calculator.xlsx
+++ b/Hardware/Arch_Bridge/Current Limit calculator.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t xml:space="preserve">A</t>
   </si>
@@ -92,6 +92,33 @@
   </si>
   <si>
     <t xml:space="preserve">int64_t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Railsync Driving load sense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rtotal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS Volts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sense Volts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"-R26 +R27”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“+R26 -R27”</t>
   </si>
 </sst>
 </file>
@@ -197,13 +224,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.88"/>
   </cols>
@@ -986,7 +1013,226 @@
         <v>OK</v>
       </c>
     </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>3000</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <f aca="false">B33*0.95</f>
+        <v>2850</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <f aca="false">B33*1.05</f>
+        <v>3150</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>22000</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <f aca="false">B34*1.05</f>
+        <v>23100</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <f aca="false">B34*0.95</f>
+        <v>20900</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <f aca="false">B34/B33</f>
+        <v>7.33333333333333</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <f aca="false">C34/C33</f>
+        <v>8.10526315789474</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <f aca="false">D34/D33</f>
+        <v>6.63492063492064</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <f aca="false">B34+B33</f>
+        <v>25000</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <f aca="false">C34+C33</f>
+        <v>25950</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <f aca="false">D34+D33</f>
+        <v>24050</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <f aca="false">$A38/B$36*B$33</f>
+        <v>0.48</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <f aca="false">$A38/C$36*C$33</f>
+        <v>0.439306358381503</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <f aca="false">$A38/D$36*D$33</f>
+        <v>0.523908523908524</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <f aca="false">ROUND($C$14*B38,0)</f>
+        <v>634</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <f aca="false">A39/$B$36*$B$33</f>
+        <v>0.6</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <f aca="false">$A39/C$36*C$33</f>
+        <v>0.549132947976879</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <f aca="false">$A39/D$36*D$33</f>
+        <v>0.654885654885655</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <f aca="false">ROUND($C$14*B39,0)</f>
+        <v>793</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <f aca="false">A40/$B$36*$B$33</f>
+        <v>0.84</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <f aca="false">$A40/C$36*C$33</f>
+        <v>0.76878612716763</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <f aca="false">$A40/D$36*D$33</f>
+        <v>0.916839916839917</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <f aca="false">ROUND($C$14*B40,0)</f>
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <f aca="false">A41/$B$36*$B$33</f>
+        <v>1.44</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <f aca="false">$A41/C$36*C$33</f>
+        <v>1.31791907514451</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <f aca="false">$A41/D$36*D$33</f>
+        <v>1.57172557172557</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <f aca="false">ROUND($C$14*B41,0)</f>
+        <v>1902</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <f aca="false">A42/$B$36*$B$33</f>
+        <v>1.8</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <f aca="false">$A42/C$36*C$33</f>
+        <v>1.64739884393064</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <f aca="false">$A42/D$36*D$33</f>
+        <v>1.96465696465696</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <f aca="false">ROUND($C$14*B42,0)</f>
+        <v>2378</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <f aca="false">A43/$B$36*$B$33</f>
+        <v>2.88</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <f aca="false">$A43/C$36*C$33</f>
+        <v>2.63583815028902</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <f aca="false">$A43/D$36*D$33</f>
+        <v>3.14345114345114</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <f aca="false">ROUND($C$14*B43,0)</f>
+        <v>3804</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A32:C32"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>